<commit_message>
type: feat Save summary
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/summary.xlsx
+++ b/POS Code/Experiments/summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zefuh\workspace\interpretability-of-source-code-transformers\POS Code\Experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuh/Documents/interpretability-of-source-code-transformers/POS Code/Experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C98BBED-CC53-40E5-B256-A4CBD62910DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08155EC-0621-5D49-8F03-481801E8377B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{BEC22610-DBDE-49A5-ABDC-7DB261D6BA7F}"/>
+    <workbookView xWindow="60" yWindow="1220" windowWidth="28800" windowHeight="15440" xr2:uid="{BEC22610-DBDE-49A5-ABDC-7DB261D6BA7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,22 +25,77 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Layer1</t>
-  </si>
-  <si>
-    <t>Layer0 (Embedding)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+  <si>
+    <t>When NAME is similar to STRING:
+For example:
+NAME: h3
+STRING: '&lt;h3&gt;'</t>
+  </si>
+  <si>
+    <t>Layer</t>
+  </si>
+  <si>
+    <t>0,1</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>STRING</t>
+  </si>
+  <si>
+    <t>0,1,2</t>
+  </si>
+  <si>
+    <t>0,1,2,3</t>
+  </si>
+  <si>
+    <t>NUMBER</t>
+  </si>
+  <si>
+    <t>KEYWORD</t>
+  </si>
+  <si>
+    <t>When NAME is similar to KEYWORD:
+The length of NAME is similar to KEYWORD</t>
+  </si>
+  <si>
+    <t>KW-&gt;NAME</t>
+  </si>
+  <si>
+    <t>NAME-&gt;STRING</t>
+  </si>
+  <si>
+    <t>Incremental Layerwise</t>
+  </si>
+  <si>
+    <t>Independent Layerwise</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -54,7 +109,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -62,12 +117,143 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,28 +568,436 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8704103-9B8A-466C-B35C-1C4C0078F27B}">
-  <dimension ref="A5:A6"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="1" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="19">
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="15">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="C6" s="9">
+        <v>1</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.996</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13">
+        <v>1</v>
+      </c>
+      <c r="C7" s="13">
+        <v>1</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="E7" s="17">
+        <v>0.624</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="23"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>0</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.99</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>1</v>
+      </c>
+      <c r="B9" s="9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="23"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <v>2</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+      <c r="C10" s="9">
+        <v>1</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0.995</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>3</v>
+      </c>
+      <c r="B11" s="13">
+        <v>1</v>
+      </c>
+      <c r="C11" s="13">
+        <v>1</v>
+      </c>
+      <c r="D11" s="13">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="E11" s="13">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="6">
+        <v>1</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="E14" s="19">
+        <v>0.34</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="9">
+        <v>0.995</v>
+      </c>
+      <c r="C15" s="9">
+        <v>1</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="E15" s="15">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="13">
+        <v>0.998</v>
+      </c>
+      <c r="C16" s="13">
+        <v>1</v>
+      </c>
+      <c r="D16" s="13">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="E16" s="17">
+        <v>0.622</v>
+      </c>
+      <c r="F16" s="21"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>0</v>
+      </c>
+      <c r="B17" s="6">
+        <v>1</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="8">
+        <v>1</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0.998</v>
+      </c>
+      <c r="C18" s="9">
+        <v>1</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0.98</v>
+      </c>
+      <c r="E18" s="9">
+        <v>0.45</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="23"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="8">
+        <v>2</v>
+      </c>
+      <c r="B19" s="9">
+        <v>0.998</v>
+      </c>
+      <c r="C19" s="9">
+        <v>1</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0.997</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>3</v>
+      </c>
+      <c r="B20" s="13">
+        <v>0.995</v>
+      </c>
+      <c r="C20" s="13">
+        <v>1</v>
+      </c>
+      <c r="D20" s="13">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="E20" s="13">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="F20" s="14"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="4"/>
+    </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="G17:H20"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:H7"/>
+    <mergeCell ref="G8:H11"/>
+    <mergeCell ref="G14:H16"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E5:E11 E14:E20">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2E3199E2-AB3D-CD46-BB7D-97AF191FF721}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:B11 B14:B20">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFD6007B"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5090F494-7BE1-2D4D-A417-D4BF4C1DFD13}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2E3199E2-AB3D-CD46-BB7D-97AF191FF721}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E5:E11 E14:E20</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5090F494-7BE1-2D4D-A417-D4BF4C1DFD13}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFD6007B"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B5:B11 B14:B20</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
type: feat Update the summary file
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/summary.xlsx
+++ b/POS Code/Experiments/summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuh/Documents/interpretability-of-source-code-transformers/POS Code/Experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08155EC-0621-5D49-8F03-481801E8377B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FCC000-C46B-D548-8C91-9D0EFCAC1FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="1220" windowWidth="28800" windowHeight="15440" xr2:uid="{BEC22610-DBDE-49A5-ABDC-7DB261D6BA7F}"/>
+    <workbookView xWindow="380" yWindow="660" windowWidth="28800" windowHeight="15440" xr2:uid="{BEC22610-DBDE-49A5-ABDC-7DB261D6BA7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>When NAME is similar to STRING:
 For example:
@@ -71,6 +71,10 @@
   </si>
   <si>
     <t>Independent Layerwise</t>
+  </si>
+  <si>
+    <t>Layer 0: Embedding layer
+Layer 1: the first attention layer</t>
   </si>
 </sst>
 </file>
@@ -204,16 +208,10 @@
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -223,7 +221,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -233,26 +230,35 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -571,28 +577,34 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
+      <c r="A2" s="19"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
+      <c r="A3" s="19"/>
     </row>
     <row r="4" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
@@ -609,162 +621,162 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="15">
         <v>0.83599999999999997</v>
       </c>
-      <c r="C5" s="6">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6">
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
         <v>0.98799999999999999</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="4">
         <v>0.91900000000000004</v>
       </c>
       <c r="F5" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="4"/>
+      <c r="H5" s="18"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="12">
         <v>0.72899999999999998</v>
       </c>
-      <c r="C6" s="9">
-        <v>1</v>
-      </c>
-      <c r="D6" s="9">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
         <v>0.996</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6">
         <v>0.89500000000000002</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="4"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="13">
-        <v>1</v>
-      </c>
-      <c r="C7" s="13">
-        <v>1</v>
-      </c>
-      <c r="D7" s="13">
+      <c r="B7" s="10">
+        <v>1</v>
+      </c>
+      <c r="C7" s="10">
+        <v>1</v>
+      </c>
+      <c r="D7" s="10">
         <v>0.97699999999999998</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="13">
         <v>0.624</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="4"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="A8" s="3">
         <v>0</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="4">
         <v>0.94799999999999995</v>
       </c>
-      <c r="C8" s="6">
-        <v>1</v>
-      </c>
-      <c r="D8" s="6">
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4">
         <v>0.98599999999999999</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="4">
         <v>0.99</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="23" t="s">
+      <c r="F8" s="5"/>
+      <c r="G8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="4"/>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="8">
-        <v>1</v>
-      </c>
-      <c r="B9" s="9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="9">
+      <c r="A9" s="6">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
         <v>0.99199999999999999</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9">
         <v>0.4</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="4"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="8">
+      <c r="A10" s="6">
         <v>2</v>
       </c>
-      <c r="B10" s="9">
-        <v>1</v>
-      </c>
-      <c r="C10" s="9">
-        <v>1</v>
-      </c>
-      <c r="D10" s="9">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
         <v>0.995</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10">
         <v>0.89500000000000002</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="4"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+      <c r="A11" s="9">
         <v>3</v>
       </c>
-      <c r="B11" s="13">
-        <v>1</v>
-      </c>
-      <c r="C11" s="13">
-        <v>1</v>
-      </c>
-      <c r="D11" s="13">
+      <c r="B11" s="10">
+        <v>1</v>
+      </c>
+      <c r="C11" s="10">
+        <v>1</v>
+      </c>
+      <c r="D11" s="10">
         <v>0.95099999999999996</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="10">
         <v>0.96199999999999997</v>
       </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="4"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B13" t="s">
@@ -781,155 +793,155 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="6">
-        <v>1</v>
-      </c>
-      <c r="C14" s="6">
-        <v>1</v>
-      </c>
-      <c r="D14" s="6">
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4">
         <v>0.96399999999999997</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="15">
         <v>0.34</v>
       </c>
       <c r="F14" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="23" t="s">
+      <c r="G14" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="4"/>
+      <c r="H14" s="18"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15">
         <v>0.995</v>
       </c>
-      <c r="C15" s="9">
-        <v>1</v>
-      </c>
-      <c r="D15" s="9">
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
         <v>0.96799999999999997</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="12">
         <v>0.57099999999999995</v>
       </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="4"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="18"/>
     </row>
     <row r="16" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="10">
         <v>0.998</v>
       </c>
-      <c r="C16" s="13">
-        <v>1</v>
-      </c>
-      <c r="D16" s="13">
+      <c r="C16" s="10">
+        <v>1</v>
+      </c>
+      <c r="D16" s="10">
         <v>0.97699999999999998</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="13">
         <v>0.622</v>
       </c>
-      <c r="F16" s="21"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="4"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="18"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
+      <c r="A17" s="3">
         <v>0</v>
       </c>
-      <c r="B17" s="6">
-        <v>1</v>
-      </c>
-      <c r="C17" s="6">
-        <v>1</v>
-      </c>
-      <c r="D17" s="6">
+      <c r="B17" s="4">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1</v>
+      </c>
+      <c r="D17" s="4">
         <v>0.91700000000000004</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="4">
         <v>0.94299999999999995</v>
       </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="23" t="s">
+      <c r="F17" s="5"/>
+      <c r="G17" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="4"/>
+      <c r="H17" s="18"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="8">
-        <v>1</v>
-      </c>
-      <c r="B18" s="9">
+      <c r="A18" s="6">
+        <v>1</v>
+      </c>
+      <c r="B18">
         <v>0.998</v>
       </c>
-      <c r="C18" s="9">
-        <v>1</v>
-      </c>
-      <c r="D18" s="9">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
         <v>0.98</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18">
         <v>0.45</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="23"/>
-      <c r="H18" s="4"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="18"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="8">
+      <c r="A19" s="6">
         <v>2</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19">
         <v>0.998</v>
       </c>
-      <c r="C19" s="9">
-        <v>1</v>
-      </c>
-      <c r="D19" s="9">
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
         <v>0.997</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19">
         <v>0.85499999999999998</v>
       </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="4"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="18"/>
     </row>
     <row r="20" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
+      <c r="A20" s="9">
         <v>3</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B20" s="10">
         <v>0.995</v>
       </c>
-      <c r="C20" s="13">
-        <v>1</v>
-      </c>
-      <c r="D20" s="13">
+      <c r="C20" s="10">
+        <v>1</v>
+      </c>
+      <c r="D20" s="10">
         <v>0.95199999999999996</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="10">
         <v>0.96199999999999997</v>
       </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="4"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="G17:H20"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="F14:F16"/>
@@ -937,6 +949,7 @@
     <mergeCell ref="G5:H7"/>
     <mergeCell ref="G8:H11"/>
     <mergeCell ref="G14:H16"/>
+    <mergeCell ref="B1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="E5:E11 E14:E20">
     <cfRule type="dataBar" priority="2">

</xml_diff>

<commit_message>
type: feat Update the summary
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/summary.xlsx
+++ b/POS Code/Experiments/summary.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuh/Documents/interpretability-of-source-code-transformers/POS Code/Experiments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zefuh\workspace\interpretability-of-source-code-transformers\POS Code\Experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FCC000-C46B-D548-8C91-9D0EFCAC1FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1BB367B-11FA-4724-8E43-3714F998DD4E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="660" windowWidth="28800" windowHeight="15440" xr2:uid="{BEC22610-DBDE-49A5-ABDC-7DB261D6BA7F}"/>
+    <workbookView xWindow="375" yWindow="660" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{BEC22610-DBDE-49A5-ABDC-7DB261D6BA7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
   <si>
     <t>When NAME is similar to STRING:
 For example:
@@ -75,6 +76,100 @@
   <si>
     <t>Layer 0: Embedding layer
 Layer 1: the first attention layer</t>
+  </si>
+  <si>
+    <t>Selection</t>
+  </si>
+  <si>
+    <t>original # of neurons</t>
+  </si>
+  <si>
+    <t>Baseline accuracy</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t># of neurons</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>LCA</t>
+  </si>
+  <si>
+    <t>Neuron reduction</t>
+  </si>
+  <si>
+    <t>Probeless</t>
+  </si>
+  <si>
+    <t>Clustering threshold</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>Layer Selection</t>
+  </si>
+  <si>
+    <t>Performance layer delta</t>
+  </si>
+  <si>
+    <t>Performance delta</t>
+  </si>
+  <si>
+    <t>Layerwise
+(LS)</t>
+  </si>
+  <si>
+    <t>LS+CC+LCA</t>
+  </si>
+  <si>
+    <t>BERT</t>
+  </si>
+  <si>
+    <t>CodeBERT</t>
+  </si>
+  <si>
+    <t>Layer 4</t>
+  </si>
+  <si>
+    <t>2-1</t>
+  </si>
+  <si>
+    <t>CodeBERTa</t>
+  </si>
+  <si>
+    <t>CodeGPTJava</t>
+  </si>
+  <si>
+    <t>CodeGPTJavaAdapted</t>
+  </si>
+  <si>
+    <t>CodeGPTPy</t>
+  </si>
+  <si>
+    <t>CodeGPTPyAdapted</t>
+  </si>
+  <si>
+    <t>GPT2</t>
+  </si>
+  <si>
+    <t>GraphCodeBERT</t>
+  </si>
+  <si>
+    <t>JavaBERT</t>
+  </si>
+  <si>
+    <t>RoBERTa</t>
+  </si>
+  <si>
+    <t>UniXCoder</t>
   </si>
 </sst>
 </file>
@@ -205,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -239,6 +334,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -259,6 +357,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -576,34 +686,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8704103-9B8A-466C-B35C-1C4C0078F27B}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:8" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="19"/>
-    </row>
-    <row r="4" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="20"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -620,7 +730,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -636,15 +746,15 @@
       <c r="E5" s="4">
         <v>0.91900000000000004</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="18"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H5" s="19"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
@@ -660,11 +770,11 @@
       <c r="E6">
         <v>0.89500000000000002</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="18"/>
-    </row>
-    <row r="7" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="22"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="19"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
@@ -683,10 +793,10 @@
       <c r="F7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="18"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G7" s="18"/>
+      <c r="H7" s="19"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>0</v>
       </c>
@@ -703,12 +813,12 @@
         <v>0.99</v>
       </c>
       <c r="F8" s="5"/>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="18"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H8" s="19"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>1</v>
       </c>
@@ -727,10 +837,10 @@
       <c r="F9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="18"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G9" s="18"/>
+      <c r="H9" s="19"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>2</v>
       </c>
@@ -747,10 +857,10 @@
         <v>0.89500000000000002</v>
       </c>
       <c r="F10" s="8"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="18"/>
-    </row>
-    <row r="11" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="18"/>
+      <c r="H10" s="19"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>3</v>
       </c>
@@ -767,15 +877,15 @@
         <v>0.96199999999999997</v>
       </c>
       <c r="F11" s="11"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
-    </row>
-    <row r="12" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="G11" s="18"/>
+      <c r="H11" s="19"/>
+    </row>
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
@@ -792,7 +902,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
@@ -808,15 +918,15 @@
       <c r="E14" s="15">
         <v>0.34</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="18"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H14" s="19"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
@@ -832,11 +942,11 @@
       <c r="E15" s="12">
         <v>0.57099999999999995</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="18"/>
-    </row>
-    <row r="16" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="22"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="19"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>6</v>
       </c>
@@ -852,11 +962,11 @@
       <c r="E16" s="13">
         <v>0.622</v>
       </c>
-      <c r="F16" s="22"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="18"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F16" s="23"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="19"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>0</v>
       </c>
@@ -873,12 +983,12 @@
         <v>0.94299999999999995</v>
       </c>
       <c r="F17" s="5"/>
-      <c r="G17" s="17" t="s">
+      <c r="G17" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="18"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H17" s="19"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>1</v>
       </c>
@@ -897,10 +1007,10 @@
       <c r="F18" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="17"/>
-      <c r="H18" s="18"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G18" s="18"/>
+      <c r="H18" s="19"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>2</v>
       </c>
@@ -917,10 +1027,10 @@
         <v>0.85499999999999998</v>
       </c>
       <c r="F19" s="8"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="18"/>
-    </row>
-    <row r="20" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="18"/>
+      <c r="H19" s="19"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <v>3</v>
       </c>
@@ -937,8 +1047,8 @@
         <v>0.96199999999999997</v>
       </c>
       <c r="F20" s="11"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1013,4 +1123,325 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8AFE0CD-28E1-4CD8-98C8-5BF45FEC86C2}">
+  <dimension ref="A1:N26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="17" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="17" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" style="17" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="17" customWidth="1"/>
+    <col min="9" max="9" width="20" style="17" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="17"/>
+    <col min="11" max="11" width="15.42578125" style="17" customWidth="1"/>
+    <col min="12" max="13" width="9.140625" style="17"/>
+    <col min="14" max="14" width="14" style="17" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="17">
+        <v>9984</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="25">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="25">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="17">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="25">
+        <v>0.97099999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="25">
+        <v>0.98299999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="26">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="25">
+        <v>0.96299999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="25">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="27">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
+      <c r="B13" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="26">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
+      <c r="B14" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="25">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="25">
+        <v>0.90700000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="19"/>
+      <c r="B17" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="19"/>
+      <c r="B18" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="17">
+        <v>3840</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="19"/>
+      <c r="B19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="25">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="19"/>
+      <c r="B20" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="25">
+        <v>0.61499999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="19"/>
+      <c r="B22" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="19"/>
+      <c r="B23" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="17">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="19"/>
+      <c r="B24" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="17">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="19"/>
+      <c r="B25" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="25">
+        <v>0.98399999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="19"/>
+      <c r="B26" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="25">
+        <v>0.98</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
type: feat Update the summary report
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/summary.xlsx
+++ b/POS Code/Experiments/summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuh/Documents/interpretability-of-source-code-transformers/POS Code/Experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C7653D-8AEE-254B-AD91-B69FE5950351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57EE23AE-020A-B042-8033-ABCC1D26BAFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="28800" windowHeight="15440" activeTab="1" xr2:uid="{BEC22610-DBDE-49A5-ABDC-7DB261D6BA7F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="43">
   <si>
     <t>Selection</t>
   </si>
@@ -165,6 +165,9 @@
   <si>
     <t>Layer 12</t>
   </si>
+  <si>
+    <t>Layer 3</t>
+  </si>
 </sst>
 </file>
 
@@ -173,7 +176,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +191,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -290,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -355,6 +364,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -373,10 +385,13 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -14387,7 +14402,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="23" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -14431,7 +14446,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="24"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
@@ -14473,7 +14488,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -14517,7 +14532,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -14559,7 +14574,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -14603,7 +14618,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="23"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
@@ -14645,7 +14660,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="24"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
@@ -14687,7 +14702,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -14731,7 +14746,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -14773,7 +14788,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
@@ -14815,7 +14830,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="23" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -14859,7 +14874,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="23"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
@@ -14901,7 +14916,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="23"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
@@ -14943,7 +14958,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
@@ -14985,7 +15000,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -15029,7 +15044,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="23"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
@@ -15071,7 +15086,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="23"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
@@ -15113,7 +15128,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="23"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="1" t="s">
         <v>6</v>
       </c>
@@ -15155,7 +15170,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="24"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="4" t="s">
         <v>8</v>
       </c>
@@ -15197,7 +15212,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="23" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -15241,7 +15256,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="23"/>
+      <c r="A22" s="24"/>
       <c r="B22" s="1" t="s">
         <v>14</v>
       </c>
@@ -15283,7 +15298,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="23"/>
+      <c r="A23" s="24"/>
       <c r="B23" s="1" t="s">
         <v>10</v>
       </c>
@@ -15325,7 +15340,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="23"/>
+      <c r="A24" s="24"/>
       <c r="B24" s="1" t="s">
         <v>5</v>
       </c>
@@ -15367,7 +15382,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="23"/>
+      <c r="A25" s="24"/>
       <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
@@ -15409,7 +15424,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="24"/>
+      <c r="A26" s="25"/>
       <c r="B26" s="4" t="s">
         <v>8</v>
       </c>
@@ -15470,7 +15485,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15484,7 +15499,7 @@
     <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.6640625" bestFit="1" customWidth="1"/>
@@ -15534,7 +15549,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="23" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -15578,14 +15593,16 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="24"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="5">
         <v>0.61570000000000003</v>
       </c>
-      <c r="D3" s="5"/>
+      <c r="D3" s="5">
+        <v>0.64019999999999999</v>
+      </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5">
         <v>0.61270000000000002</v>
@@ -15593,16 +15610,26 @@
       <c r="G3" s="5">
         <v>0.51390000000000002</v>
       </c>
-      <c r="H3" s="5"/>
+      <c r="H3" s="5">
+        <v>0.63580000000000003</v>
+      </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="6"/>
+      <c r="K3" s="5">
+        <v>0.63870000000000005</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0.57279999999999998</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0.4839</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0.66800000000000004</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -15646,7 +15673,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -15664,7 +15691,7 @@
       <c r="N5" s="6"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -15673,7 +15700,9 @@
       <c r="C6" s="2">
         <v>29</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2">
+        <v>79</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2">
         <v>9</v>
@@ -15681,23 +15710,37 @@
       <c r="G6" s="2">
         <v>29</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="H6" s="2">
+        <v>79</v>
+      </c>
+      <c r="I6" s="2">
+        <v>19</v>
+      </c>
       <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="3"/>
+      <c r="K6" s="2">
+        <v>489</v>
+      </c>
+      <c r="L6" s="2">
+        <v>39</v>
+      </c>
+      <c r="M6" s="2">
+        <v>9</v>
+      </c>
+      <c r="N6" s="3">
+        <v>29</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="23"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="7">
         <v>0.61599999999999999</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="7">
+        <v>0.64239999999999997</v>
+      </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7">
         <v>0.58819999999999995</v>
@@ -15705,43 +15748,76 @@
       <c r="G7" s="7">
         <v>0.60809999999999997</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="H7" s="7">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="I7" s="7">
+        <v>0.61099999999999999</v>
+      </c>
       <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="8"/>
+      <c r="K7" s="28">
+        <v>0.62590000000000001</v>
+      </c>
+      <c r="L7" s="28">
+        <v>0.5706</v>
+      </c>
+      <c r="M7" s="28">
+        <v>0.5696</v>
+      </c>
+      <c r="N7" s="8">
+        <v>0.65300000000000002</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="24"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="5">
         <f>1-C6/C2</f>
         <v>0.99709535256410253</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28">
-        <f t="shared" ref="D8:G8" si="0">1-F6/F2</f>
+      <c r="D8" s="5">
+        <f>1-D6/D2</f>
+        <v>0.99208733974358976</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5">
+        <f t="shared" ref="F8:N8" si="0">1-F6/F2</f>
         <v>0.99909855769230771</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="5">
         <f t="shared" si="0"/>
         <v>0.99709535256410253</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="6"/>
+      <c r="H8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.99208733974358976</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.99809695512820518</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.95102163461538458</v>
+      </c>
+      <c r="L8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.99609375</v>
+      </c>
+      <c r="M8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.99909855769230771</v>
+      </c>
+      <c r="N8" s="6">
+        <f t="shared" si="0"/>
+        <v>0.99709535256410253</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -15761,7 +15837,7 @@
       <c r="N9" s="3"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -15779,7 +15855,7 @@
       <c r="N10" s="18"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
@@ -15797,7 +15873,7 @@
       <c r="N11" s="19"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="23" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -15806,66 +15882,114 @@
       <c r="C12" s="9">
         <v>-1</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2">
+        <v>0.7</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2">
         <v>0.6</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
+      <c r="G12" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.6</v>
+      </c>
       <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="3"/>
+      <c r="K12" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0.2</v>
+      </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="23"/>
+    <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="24"/>
       <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="17">
         <v>29</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1">
+        <v>1742</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1">
         <v>1023</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="G13" s="1">
+        <v>623</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1023</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1283</v>
+      </c>
       <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="11"/>
+      <c r="K13" s="1">
+        <v>2555</v>
+      </c>
+      <c r="L13" s="1">
+        <v>843</v>
+      </c>
+      <c r="M13" s="1">
+        <v>1977</v>
+      </c>
+      <c r="N13" s="31">
+        <v>8890</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="23"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="7">
         <v>0.62960000000000005</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="7">
+        <v>0.6552</v>
+      </c>
       <c r="E14" s="7"/>
-      <c r="F14" s="27">
+      <c r="F14" s="7">
         <v>0.62590000000000001</v>
       </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="15"/>
+      <c r="G14" s="7">
+        <v>0.64129999999999998</v>
+      </c>
+      <c r="H14" s="7">
+        <v>0.62590000000000001</v>
+      </c>
+      <c r="I14" s="28">
+        <v>0.62170000000000003</v>
+      </c>
       <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="8"/>
+      <c r="K14" s="7">
+        <v>0.64349999999999996</v>
+      </c>
+      <c r="L14" s="7">
+        <v>0.58420000000000005</v>
+      </c>
+      <c r="M14" s="7">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="N14" s="8">
+        <v>0.67020000000000002</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
@@ -15873,32 +15997,58 @@
         <f>1-C13/C2</f>
         <v>0.99709535256410253</v>
       </c>
-      <c r="D15" s="5"/>
+      <c r="D15" s="5">
+        <f>1-D13/D2</f>
+        <v>0.82552083333333337</v>
+      </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5">
-        <f t="shared" ref="D15:F15" si="1">1-F13/F2</f>
+        <f t="shared" ref="F15:N15" si="1">1-F13/F2</f>
         <v>0.89753605769230771</v>
       </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="16"/>
+      <c r="G15" s="5">
+        <f t="shared" si="1"/>
+        <v>0.93760016025641024</v>
+      </c>
+      <c r="H15" s="5">
+        <f t="shared" si="1"/>
+        <v>0.89753605769230771</v>
+      </c>
+      <c r="I15" s="5">
+        <f t="shared" si="1"/>
+        <v>0.87149439102564097</v>
+      </c>
       <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="6"/>
+      <c r="K15" s="5">
+        <f t="shared" si="1"/>
+        <v>0.74409054487179493</v>
+      </c>
+      <c r="L15" s="5">
+        <f t="shared" si="1"/>
+        <v>0.91556490384615385</v>
+      </c>
+      <c r="M15" s="5">
+        <f t="shared" si="1"/>
+        <v>0.80198317307692313</v>
+      </c>
+      <c r="N15" s="6">
+        <f t="shared" si="1"/>
+        <v>0.10957532051282048</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
         <v>41</v>
@@ -15906,23 +16056,37 @@
       <c r="G16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
+      <c r="H16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="3"/>
+      <c r="K16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="23"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="1">
         <v>3</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1">
         <v>3</v>
@@ -15930,16 +16094,28 @@
       <c r="G17" s="1">
         <v>3</v>
       </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="H17" s="1">
+        <v>3</v>
+      </c>
+      <c r="I17" s="1">
+        <v>3</v>
+      </c>
       <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="11"/>
+      <c r="K17" s="1">
+        <v>3</v>
+      </c>
+      <c r="L17" s="1">
+        <v>3</v>
+      </c>
+      <c r="M17" s="1">
+        <v>3</v>
+      </c>
+      <c r="N17" s="11">
+        <v>3</v>
+      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="23"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
@@ -15947,7 +16123,10 @@
         <f>12*768</f>
         <v>9216</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="1">
+        <f>13*768</f>
+        <v>9984</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1">
         <f>13*768</f>
@@ -15957,40 +16136,68 @@
         <f>1*768</f>
         <v>768</v>
       </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="H18" s="1">
+        <v>9984</v>
+      </c>
+      <c r="I18" s="1">
+        <f>8*768</f>
+        <v>6144</v>
+      </c>
       <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="11"/>
+      <c r="K18" s="1">
+        <v>9984</v>
+      </c>
+      <c r="L18" s="1">
+        <f>3*768</f>
+        <v>2304</v>
+      </c>
+      <c r="M18" s="1">
+        <v>768</v>
+      </c>
+      <c r="N18" s="11">
+        <v>9984</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="23"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="7">
         <v>0.74199999999999999</v>
       </c>
-      <c r="D19" s="7"/>
+      <c r="D19" s="7">
+        <v>0.83320000000000005</v>
+      </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7">
         <v>0.69989999999999997</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19" s="7">
         <v>0.56269999999999998</v>
       </c>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="H19" s="7">
+        <v>0.70720000000000005</v>
+      </c>
+      <c r="I19" s="7">
+        <v>0.65049999999999997</v>
+      </c>
       <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="8"/>
+      <c r="K19" s="7">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="L19" s="7">
+        <v>0.59240000000000004</v>
+      </c>
+      <c r="M19" s="7">
+        <v>0.56269999999999998</v>
+      </c>
+      <c r="N19" s="8">
+        <v>0.73650000000000004</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="24"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="4" t="s">
         <v>8</v>
       </c>
@@ -15998,26 +16205,47 @@
         <f>1-C18/C2</f>
         <v>7.6923076923076872E-2</v>
       </c>
-      <c r="D20" s="5"/>
+      <c r="D20" s="5">
+        <f>1-D18/D2</f>
+        <v>0</v>
+      </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5">
-        <f t="shared" ref="D20:G20" si="2">1-F18/F2</f>
+        <f t="shared" ref="F20:N20" si="2">1-F18/F2</f>
         <v>0</v>
       </c>
       <c r="G20" s="5">
         <f t="shared" si="2"/>
         <v>0.92307692307692313</v>
       </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+      <c r="H20" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="5">
+        <f t="shared" si="2"/>
+        <v>0.38461538461538458</v>
+      </c>
       <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="6"/>
+      <c r="K20" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L20" s="5">
+        <f t="shared" si="2"/>
+        <v>0.76923076923076916</v>
+      </c>
+      <c r="M20" s="5">
+        <f t="shared" si="2"/>
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="N20" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="23" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -16026,7 +16254,9 @@
       <c r="C21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
         <v>41</v>
@@ -16034,23 +16264,37 @@
       <c r="G21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
+      <c r="H21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="3"/>
+      <c r="K21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="23"/>
+      <c r="A22" s="24"/>
       <c r="B22" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="12"/>
+      <c r="D22" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="E22" s="12"/>
       <c r="F22" s="12" t="s">
         <v>36</v>
@@ -16058,23 +16302,37 @@
       <c r="G22" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
+      <c r="H22" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="13"/>
+      <c r="K22" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="M22" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="N22" s="13" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="23"/>
+      <c r="A23" s="24"/>
       <c r="B23" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C23" s="1">
         <v>-1</v>
       </c>
-      <c r="D23" s="1"/>
+      <c r="D23" s="1">
+        <v>-1</v>
+      </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1">
         <v>-1</v>
@@ -16082,23 +16340,37 @@
       <c r="G23" s="1">
         <v>-1</v>
       </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="H23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I23" s="1">
+        <v>-1</v>
+      </c>
       <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="11"/>
+      <c r="K23" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N23" s="11">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="23"/>
+    <row r="24" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="24"/>
       <c r="B24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="1">
         <v>29</v>
       </c>
-      <c r="D24" s="1"/>
+      <c r="D24" s="1">
+        <v>99</v>
+      </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1">
         <v>49</v>
@@ -16106,64 +16378,111 @@
       <c r="G24" s="1">
         <v>9</v>
       </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
+      <c r="H24" s="1">
+        <v>199</v>
+      </c>
+      <c r="I24" s="1">
+        <v>199</v>
+      </c>
       <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="11"/>
+      <c r="K24" s="30">
+        <v>399</v>
+      </c>
+      <c r="L24" s="1">
+        <v>99</v>
+      </c>
+      <c r="M24" s="1">
+        <v>9</v>
+      </c>
+      <c r="N24" s="11">
+        <v>29</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="23"/>
+      <c r="A25" s="24"/>
       <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="27">
+      <c r="C25" s="7">
         <v>0.61380000000000001</v>
       </c>
-      <c r="D25" s="7"/>
+      <c r="D25" s="7">
+        <v>0.65149999999999997</v>
+      </c>
       <c r="E25" s="15"/>
-      <c r="F25" s="27">
+      <c r="F25" s="7">
         <v>0.61050000000000004</v>
       </c>
-      <c r="G25" s="27">
+      <c r="G25" s="7">
         <v>0.5655</v>
       </c>
-      <c r="H25" s="15"/>
-      <c r="I25" s="14"/>
+      <c r="H25" s="28">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="I25" s="14">
+        <v>0.61119999999999997</v>
+      </c>
       <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="18"/>
+      <c r="K25" s="7">
+        <v>0.63649999999999995</v>
+      </c>
+      <c r="L25" s="28">
+        <v>0.57869999999999999</v>
+      </c>
+      <c r="M25" s="28">
+        <v>0.5655</v>
+      </c>
+      <c r="N25" s="29">
+        <v>0.65559999999999996</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="24"/>
+      <c r="A26" s="25"/>
       <c r="B26" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="28">
+      <c r="C26" s="5">
         <f>1-C24/C2</f>
         <v>0.99709535256410253</v>
       </c>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28">
-        <f t="shared" ref="D26:G26" si="3">1-F24/F2</f>
+      <c r="D26" s="5">
+        <f>1-D24/D2</f>
+        <v>0.99008413461538458</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5">
+        <f t="shared" ref="F26:N26" si="3">1-F24/F2</f>
         <v>0.99509214743589747</v>
       </c>
-      <c r="G26" s="28">
+      <c r="G26" s="5">
         <f t="shared" si="3"/>
         <v>0.99909855769230771</v>
       </c>
-      <c r="H26" s="16"/>
-      <c r="I26" s="5"/>
+      <c r="H26" s="5">
+        <f t="shared" si="3"/>
+        <v>0.98006810897435903</v>
+      </c>
+      <c r="I26" s="5">
+        <f t="shared" si="3"/>
+        <v>0.98006810897435903</v>
+      </c>
       <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="19"/>
+      <c r="K26" s="5">
+        <f t="shared" si="3"/>
+        <v>0.96003605769230771</v>
+      </c>
+      <c r="L26" s="5">
+        <f t="shared" si="3"/>
+        <v>0.99008413461538458</v>
+      </c>
+      <c r="M26" s="5">
+        <f t="shared" si="3"/>
+        <v>0.99909855769230771</v>
+      </c>
+      <c r="N26" s="6">
+        <f t="shared" si="3"/>
+        <v>0.99709535256410253</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -16183,7 +16502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F291A794-F81B-A94A-B246-9FC1326ED183}">
   <dimension ref="A1:N111"/>
   <sheetViews>
-    <sheetView topLeftCell="A102" workbookViewId="0">
+    <sheetView topLeftCell="A38" workbookViewId="0">
       <selection activeCell="O130" sqref="O130"/>
     </sheetView>
   </sheetViews>
@@ -16233,7 +16552,7 @@
       <c r="C2" s="21">
         <v>0.94899999999999995</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="27" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="1">
@@ -16245,7 +16564,7 @@
       <c r="H2" s="21">
         <v>0.89500000000000002</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="27" t="s">
         <v>18</v>
       </c>
       <c r="K2" s="1">
@@ -16257,7 +16576,7 @@
       <c r="M2" s="21">
         <v>0.91100000000000003</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="N2" s="27" t="s">
         <v>21</v>
       </c>
     </row>
@@ -16271,7 +16590,7 @@
       <c r="C3" s="21">
         <v>0.84</v>
       </c>
-      <c r="D3" s="26"/>
+      <c r="D3" s="27"/>
       <c r="F3" s="1">
         <v>1</v>
       </c>
@@ -16281,7 +16600,7 @@
       <c r="H3" s="21">
         <v>0.93100000000000005</v>
       </c>
-      <c r="I3" s="26"/>
+      <c r="I3" s="27"/>
       <c r="K3" s="1">
         <v>1</v>
       </c>
@@ -16291,7 +16610,7 @@
       <c r="M3" s="21">
         <v>0.90900000000000003</v>
       </c>
-      <c r="N3" s="26"/>
+      <c r="N3" s="27"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -16303,7 +16622,7 @@
       <c r="C4" s="21">
         <v>0.876</v>
       </c>
-      <c r="D4" s="26"/>
+      <c r="D4" s="27"/>
       <c r="F4" s="1">
         <v>2</v>
       </c>
@@ -16313,7 +16632,7 @@
       <c r="H4" s="21">
         <v>0.873</v>
       </c>
-      <c r="I4" s="26"/>
+      <c r="I4" s="27"/>
       <c r="K4" s="1">
         <v>2</v>
       </c>
@@ -16323,7 +16642,7 @@
       <c r="M4" s="21">
         <v>0.90100000000000002</v>
       </c>
-      <c r="N4" s="26"/>
+      <c r="N4" s="27"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -16335,7 +16654,7 @@
       <c r="C5" s="21">
         <v>0.93600000000000005</v>
       </c>
-      <c r="D5" s="26"/>
+      <c r="D5" s="27"/>
       <c r="F5" s="1">
         <v>3</v>
       </c>
@@ -16345,7 +16664,7 @@
       <c r="H5" s="21">
         <v>0.83799999999999997</v>
       </c>
-      <c r="I5" s="26"/>
+      <c r="I5" s="27"/>
       <c r="K5" s="1">
         <v>3</v>
       </c>
@@ -16355,7 +16674,7 @@
       <c r="M5" s="21">
         <v>0.88400000000000001</v>
       </c>
-      <c r="N5" s="26"/>
+      <c r="N5" s="27"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -16367,7 +16686,7 @@
       <c r="C6" s="21">
         <v>0.97</v>
       </c>
-      <c r="D6" s="26"/>
+      <c r="D6" s="27"/>
       <c r="F6" s="1">
         <v>4</v>
       </c>
@@ -16377,7 +16696,7 @@
       <c r="H6" s="21">
         <v>0.97799999999999998</v>
       </c>
-      <c r="I6" s="26"/>
+      <c r="I6" s="27"/>
       <c r="K6" s="1">
         <v>4</v>
       </c>
@@ -16387,7 +16706,7 @@
       <c r="M6" s="21">
         <v>0.93899999999999995</v>
       </c>
-      <c r="N6" s="26"/>
+      <c r="N6" s="27"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -16399,7 +16718,7 @@
       <c r="C7" s="21">
         <v>0.97199999999999998</v>
       </c>
-      <c r="D7" s="26"/>
+      <c r="D7" s="27"/>
       <c r="F7" s="1">
         <v>5</v>
       </c>
@@ -16409,7 +16728,7 @@
       <c r="H7" s="21">
         <v>0.97899999999999998</v>
       </c>
-      <c r="I7" s="26"/>
+      <c r="I7" s="27"/>
       <c r="K7" s="1">
         <v>5</v>
       </c>
@@ -16419,7 +16738,7 @@
       <c r="M7" s="21">
         <v>0.91700000000000004</v>
       </c>
-      <c r="N7" s="26"/>
+      <c r="N7" s="27"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -16431,7 +16750,7 @@
       <c r="C8" s="21">
         <v>0.97399999999999998</v>
       </c>
-      <c r="D8" s="26"/>
+      <c r="D8" s="27"/>
       <c r="F8" s="1">
         <v>6</v>
       </c>
@@ -16441,7 +16760,7 @@
       <c r="H8" s="21">
         <v>0.97199999999999998</v>
       </c>
-      <c r="I8" s="26"/>
+      <c r="I8" s="27"/>
       <c r="K8" s="1">
         <v>6</v>
       </c>
@@ -16451,7 +16770,7 @@
       <c r="M8" s="21">
         <v>0.92300000000000004</v>
       </c>
-      <c r="N8" s="26"/>
+      <c r="N8" s="27"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -16463,7 +16782,7 @@
       <c r="C9" s="21">
         <v>0.97799999999999998</v>
       </c>
-      <c r="D9" s="26"/>
+      <c r="D9" s="27"/>
       <c r="F9" s="1">
         <v>7</v>
       </c>
@@ -16473,7 +16792,7 @@
       <c r="H9" s="21">
         <v>0.96499999999999997</v>
       </c>
-      <c r="I9" s="26"/>
+      <c r="I9" s="27"/>
       <c r="K9" s="1"/>
       <c r="L9" s="21"/>
       <c r="M9" s="21"/>
@@ -16489,7 +16808,7 @@
       <c r="C10" s="21">
         <v>0.97799999999999998</v>
       </c>
-      <c r="D10" s="26"/>
+      <c r="D10" s="27"/>
       <c r="F10" s="1">
         <v>8</v>
       </c>
@@ -16499,7 +16818,7 @@
       <c r="H10" s="21">
         <v>0.94899999999999995</v>
       </c>
-      <c r="I10" s="26"/>
+      <c r="I10" s="27"/>
       <c r="K10" s="1"/>
       <c r="L10" s="21"/>
       <c r="M10" s="21"/>
@@ -16515,7 +16834,7 @@
       <c r="C11" s="21">
         <v>0.97799999999999998</v>
       </c>
-      <c r="D11" s="26"/>
+      <c r="D11" s="27"/>
       <c r="F11" s="1">
         <v>9</v>
       </c>
@@ -16525,7 +16844,7 @@
       <c r="H11" s="21">
         <v>0.93</v>
       </c>
-      <c r="I11" s="26"/>
+      <c r="I11" s="27"/>
       <c r="K11" s="1"/>
       <c r="L11" s="21"/>
       <c r="M11" s="21"/>
@@ -16541,7 +16860,7 @@
       <c r="C12" s="21">
         <v>0.98099999999999998</v>
       </c>
-      <c r="D12" s="26"/>
+      <c r="D12" s="27"/>
       <c r="F12" s="1">
         <v>10</v>
       </c>
@@ -16551,7 +16870,7 @@
       <c r="H12" s="21">
         <v>0.91500000000000004</v>
       </c>
-      <c r="I12" s="26"/>
+      <c r="I12" s="27"/>
       <c r="K12" s="1"/>
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
@@ -16567,7 +16886,7 @@
       <c r="C13" s="21">
         <v>0.97899999999999998</v>
       </c>
-      <c r="D13" s="26"/>
+      <c r="D13" s="27"/>
       <c r="F13" s="1">
         <v>11</v>
       </c>
@@ -16577,7 +16896,7 @@
       <c r="H13" s="21">
         <v>0.91500000000000004</v>
       </c>
-      <c r="I13" s="26"/>
+      <c r="I13" s="27"/>
       <c r="K13" s="1"/>
       <c r="L13" s="21"/>
       <c r="M13" s="21"/>
@@ -16593,7 +16912,7 @@
       <c r="C14" s="21">
         <v>0.97399999999999998</v>
       </c>
-      <c r="D14" s="26"/>
+      <c r="D14" s="27"/>
       <c r="F14" s="1">
         <v>12</v>
       </c>
@@ -16603,7 +16922,7 @@
       <c r="H14" s="21">
         <v>0.91900000000000004</v>
       </c>
-      <c r="I14" s="26"/>
+      <c r="I14" s="27"/>
       <c r="K14" s="1"/>
       <c r="L14" s="21"/>
       <c r="M14" s="21"/>
@@ -16648,7 +16967,7 @@
       <c r="C34" s="21">
         <v>0.98199999999999998</v>
       </c>
-      <c r="D34" s="26" t="s">
+      <c r="D34" s="27" t="s">
         <v>22</v>
       </c>
       <c r="F34" s="1">
@@ -16660,7 +16979,7 @@
       <c r="H34" s="21">
         <v>0.98899999999999999</v>
       </c>
-      <c r="I34" s="26" t="s">
+      <c r="I34" s="27" t="s">
         <v>23</v>
       </c>
       <c r="K34" s="1">
@@ -16672,7 +16991,7 @@
       <c r="M34" s="21">
         <v>0.99399999999999999</v>
       </c>
-      <c r="N34" s="26" t="s">
+      <c r="N34" s="27" t="s">
         <v>24</v>
       </c>
     </row>
@@ -16686,7 +17005,7 @@
       <c r="C35" s="21">
         <v>0.91800000000000004</v>
       </c>
-      <c r="D35" s="26"/>
+      <c r="D35" s="27"/>
       <c r="F35" s="1">
         <v>1</v>
       </c>
@@ -16696,7 +17015,7 @@
       <c r="H35" s="21">
         <v>0.96399999999999997</v>
       </c>
-      <c r="I35" s="26"/>
+      <c r="I35" s="27"/>
       <c r="K35" s="1">
         <v>1</v>
       </c>
@@ -16706,7 +17025,7 @@
       <c r="M35" s="21">
         <v>0.99099999999999999</v>
       </c>
-      <c r="N35" s="26"/>
+      <c r="N35" s="27"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
@@ -16718,7 +17037,7 @@
       <c r="C36" s="21">
         <v>0.91900000000000004</v>
       </c>
-      <c r="D36" s="26"/>
+      <c r="D36" s="27"/>
       <c r="F36" s="1">
         <v>2</v>
       </c>
@@ -16728,7 +17047,7 @@
       <c r="H36" s="21">
         <v>0.97</v>
       </c>
-      <c r="I36" s="26"/>
+      <c r="I36" s="27"/>
       <c r="K36" s="1">
         <v>2</v>
       </c>
@@ -16738,7 +17057,7 @@
       <c r="M36" s="21">
         <v>0.98299999999999998</v>
       </c>
-      <c r="N36" s="26"/>
+      <c r="N36" s="27"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
@@ -16750,7 +17069,7 @@
       <c r="C37" s="21">
         <v>0.97899999999999998</v>
       </c>
-      <c r="D37" s="26"/>
+      <c r="D37" s="27"/>
       <c r="F37" s="1">
         <v>3</v>
       </c>
@@ -16760,7 +17079,7 @@
       <c r="H37" s="21">
         <v>0.96599999999999997</v>
       </c>
-      <c r="I37" s="26"/>
+      <c r="I37" s="27"/>
       <c r="K37" s="1">
         <v>3</v>
       </c>
@@ -16770,7 +17089,7 @@
       <c r="M37" s="21">
         <v>0.98</v>
       </c>
-      <c r="N37" s="26"/>
+      <c r="N37" s="27"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
@@ -16782,7 +17101,7 @@
       <c r="C38" s="21">
         <v>0.97699999999999998</v>
       </c>
-      <c r="D38" s="26"/>
+      <c r="D38" s="27"/>
       <c r="F38" s="1">
         <v>4</v>
       </c>
@@ -16792,7 +17111,7 @@
       <c r="H38" s="21">
         <v>0.96799999999999997</v>
       </c>
-      <c r="I38" s="26"/>
+      <c r="I38" s="27"/>
       <c r="K38" s="1">
         <v>4</v>
       </c>
@@ -16802,7 +17121,7 @@
       <c r="M38" s="21">
         <v>0.97099999999999997</v>
       </c>
-      <c r="N38" s="26"/>
+      <c r="N38" s="27"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
@@ -16814,7 +17133,7 @@
       <c r="C39" s="21">
         <v>0.98199999999999998</v>
       </c>
-      <c r="D39" s="26"/>
+      <c r="D39" s="27"/>
       <c r="F39" s="1">
         <v>5</v>
       </c>
@@ -16824,7 +17143,7 @@
       <c r="H39" s="21">
         <v>0.96699999999999997</v>
       </c>
-      <c r="I39" s="26"/>
+      <c r="I39" s="27"/>
       <c r="K39" s="1">
         <v>5</v>
       </c>
@@ -16834,7 +17153,7 @@
       <c r="M39" s="21">
         <v>0.873</v>
       </c>
-      <c r="N39" s="26"/>
+      <c r="N39" s="27"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
@@ -16846,7 +17165,7 @@
       <c r="C40" s="21">
         <v>0.94399999999999995</v>
       </c>
-      <c r="D40" s="26"/>
+      <c r="D40" s="27"/>
       <c r="F40" s="1">
         <v>6</v>
       </c>
@@ -16856,7 +17175,7 @@
       <c r="H40" s="21">
         <v>0.96399999999999997</v>
       </c>
-      <c r="I40" s="26"/>
+      <c r="I40" s="27"/>
       <c r="K40" s="1">
         <v>6</v>
       </c>
@@ -16866,7 +17185,7 @@
       <c r="M40" s="21">
         <v>0.97899999999999998</v>
       </c>
-      <c r="N40" s="26"/>
+      <c r="N40" s="27"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
@@ -16878,7 +17197,7 @@
       <c r="C41" s="21">
         <v>0.99299999999999999</v>
       </c>
-      <c r="D41" s="26"/>
+      <c r="D41" s="27"/>
       <c r="F41" s="1">
         <v>7</v>
       </c>
@@ -16888,7 +17207,7 @@
       <c r="H41" s="21">
         <v>0.97399999999999998</v>
       </c>
-      <c r="I41" s="26"/>
+      <c r="I41" s="27"/>
       <c r="K41" s="1">
         <v>7</v>
       </c>
@@ -16898,7 +17217,7 @@
       <c r="M41" s="21">
         <v>0.93</v>
       </c>
-      <c r="N41" s="26"/>
+      <c r="N41" s="27"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
@@ -16910,7 +17229,7 @@
       <c r="C42" s="21">
         <v>0.94599999999999995</v>
       </c>
-      <c r="D42" s="26"/>
+      <c r="D42" s="27"/>
       <c r="F42" s="1">
         <v>8</v>
       </c>
@@ -16920,7 +17239,7 @@
       <c r="H42" s="21">
         <v>0.82099999999999995</v>
       </c>
-      <c r="I42" s="26"/>
+      <c r="I42" s="27"/>
       <c r="K42" s="1">
         <v>8</v>
       </c>
@@ -16930,7 +17249,7 @@
       <c r="M42" s="21">
         <v>0.98699999999999999</v>
       </c>
-      <c r="N42" s="26"/>
+      <c r="N42" s="27"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
@@ -16942,7 +17261,7 @@
       <c r="C43" s="21">
         <v>0.98099999999999998</v>
       </c>
-      <c r="D43" s="26"/>
+      <c r="D43" s="27"/>
       <c r="F43" s="1">
         <v>9</v>
       </c>
@@ -16952,7 +17271,7 @@
       <c r="H43" s="21">
         <v>0.82799999999999996</v>
       </c>
-      <c r="I43" s="26"/>
+      <c r="I43" s="27"/>
       <c r="K43" s="1">
         <v>9</v>
       </c>
@@ -16962,7 +17281,7 @@
       <c r="M43" s="21">
         <v>0.93500000000000005</v>
       </c>
-      <c r="N43" s="26"/>
+      <c r="N43" s="27"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
@@ -16974,7 +17293,7 @@
       <c r="C44" s="21">
         <v>0.98399999999999999</v>
       </c>
-      <c r="D44" s="26"/>
+      <c r="D44" s="27"/>
       <c r="F44" s="1">
         <v>10</v>
       </c>
@@ -16984,7 +17303,7 @@
       <c r="H44" s="21">
         <v>0.84099999999999997</v>
       </c>
-      <c r="I44" s="26"/>
+      <c r="I44" s="27"/>
       <c r="K44" s="1">
         <v>10</v>
       </c>
@@ -16994,7 +17313,7 @@
       <c r="M44" s="21">
         <v>0.92500000000000004</v>
       </c>
-      <c r="N44" s="26"/>
+      <c r="N44" s="27"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
@@ -17006,7 +17325,7 @@
       <c r="C45" s="21">
         <v>0.95299999999999996</v>
       </c>
-      <c r="D45" s="26"/>
+      <c r="D45" s="27"/>
       <c r="F45" s="1">
         <v>11</v>
       </c>
@@ -17016,7 +17335,7 @@
       <c r="H45" s="21">
         <v>0.98</v>
       </c>
-      <c r="I45" s="26"/>
+      <c r="I45" s="27"/>
       <c r="K45" s="1">
         <v>11</v>
       </c>
@@ -17026,7 +17345,7 @@
       <c r="M45" s="21">
         <v>0.92400000000000004</v>
       </c>
-      <c r="N45" s="26"/>
+      <c r="N45" s="27"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
@@ -17038,7 +17357,7 @@
       <c r="C46" s="21">
         <v>0.92100000000000004</v>
       </c>
-      <c r="D46" s="26"/>
+      <c r="D46" s="27"/>
       <c r="F46" s="1">
         <v>12</v>
       </c>
@@ -17048,7 +17367,7 @@
       <c r="H46" s="21">
         <v>0.84</v>
       </c>
-      <c r="I46" s="26"/>
+      <c r="I46" s="27"/>
       <c r="K46" s="1">
         <v>12</v>
       </c>
@@ -17058,7 +17377,7 @@
       <c r="M46" s="21">
         <v>0.93300000000000005</v>
       </c>
-      <c r="N46" s="26"/>
+      <c r="N46" s="27"/>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
@@ -17099,7 +17418,7 @@
       <c r="C67" s="21">
         <v>0.77700000000000002</v>
       </c>
-      <c r="D67" s="26" t="s">
+      <c r="D67" s="27" t="s">
         <v>25</v>
       </c>
       <c r="F67" s="1">
@@ -17111,7 +17430,7 @@
       <c r="H67" s="21">
         <v>0.75900000000000001</v>
       </c>
-      <c r="I67" s="26" t="s">
+      <c r="I67" s="27" t="s">
         <v>26</v>
       </c>
       <c r="K67" s="1">
@@ -17123,7 +17442,7 @@
       <c r="M67" s="21">
         <v>0.89400000000000002</v>
       </c>
-      <c r="N67" s="26" t="s">
+      <c r="N67" s="27" t="s">
         <v>27</v>
       </c>
     </row>
@@ -17137,7 +17456,7 @@
       <c r="C68" s="21">
         <v>0.85099999999999998</v>
       </c>
-      <c r="D68" s="26"/>
+      <c r="D68" s="27"/>
       <c r="F68" s="1">
         <v>1</v>
       </c>
@@ -17147,7 +17466,7 @@
       <c r="H68" s="21">
         <v>0.97399999999999998</v>
       </c>
-      <c r="I68" s="26"/>
+      <c r="I68" s="27"/>
       <c r="K68" s="1">
         <v>1</v>
       </c>
@@ -17157,7 +17476,7 @@
       <c r="M68" s="21">
         <v>0.94299999999999995</v>
       </c>
-      <c r="N68" s="26"/>
+      <c r="N68" s="27"/>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
@@ -17169,7 +17488,7 @@
       <c r="C69" s="21">
         <v>0.93300000000000005</v>
       </c>
-      <c r="D69" s="26"/>
+      <c r="D69" s="27"/>
       <c r="F69" s="1">
         <v>2</v>
       </c>
@@ -17179,7 +17498,7 @@
       <c r="H69" s="21">
         <v>0.81899999999999995</v>
       </c>
-      <c r="I69" s="26"/>
+      <c r="I69" s="27"/>
       <c r="K69" s="1">
         <v>2</v>
       </c>
@@ -17189,7 +17508,7 @@
       <c r="M69" s="21">
         <v>0.97799999999999998</v>
       </c>
-      <c r="N69" s="26"/>
+      <c r="N69" s="27"/>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
@@ -17201,7 +17520,7 @@
       <c r="C70" s="21">
         <v>0.92700000000000005</v>
       </c>
-      <c r="D70" s="26"/>
+      <c r="D70" s="27"/>
       <c r="F70" s="1">
         <v>3</v>
       </c>
@@ -17211,7 +17530,7 @@
       <c r="H70" s="21">
         <v>0.97199999999999998</v>
       </c>
-      <c r="I70" s="26"/>
+      <c r="I70" s="27"/>
       <c r="K70" s="1">
         <v>3</v>
       </c>
@@ -17221,7 +17540,7 @@
       <c r="M70" s="21">
         <v>0.97499999999999998</v>
       </c>
-      <c r="N70" s="26"/>
+      <c r="N70" s="27"/>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
@@ -17233,7 +17552,7 @@
       <c r="C71" s="21">
         <v>0.90600000000000003</v>
       </c>
-      <c r="D71" s="26"/>
+      <c r="D71" s="27"/>
       <c r="F71" s="1">
         <v>4</v>
       </c>
@@ -17243,7 +17562,7 @@
       <c r="H71" s="21">
         <v>0.96899999999999997</v>
       </c>
-      <c r="I71" s="26"/>
+      <c r="I71" s="27"/>
       <c r="K71" s="1">
         <v>4</v>
       </c>
@@ -17253,7 +17572,7 @@
       <c r="M71" s="21">
         <v>0.85199999999999998</v>
       </c>
-      <c r="N71" s="26"/>
+      <c r="N71" s="27"/>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
@@ -17265,7 +17584,7 @@
       <c r="C72" s="21">
         <v>0.92</v>
       </c>
-      <c r="D72" s="26"/>
+      <c r="D72" s="27"/>
       <c r="F72" s="1">
         <v>5</v>
       </c>
@@ -17275,7 +17594,7 @@
       <c r="H72" s="21">
         <v>0.96499999999999997</v>
       </c>
-      <c r="I72" s="26"/>
+      <c r="I72" s="27"/>
       <c r="K72" s="1">
         <v>5</v>
       </c>
@@ -17285,7 +17604,7 @@
       <c r="M72" s="21">
         <v>0.86899999999999999</v>
       </c>
-      <c r="N72" s="26"/>
+      <c r="N72" s="27"/>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
@@ -17297,7 +17616,7 @@
       <c r="C73" s="21">
         <v>0.96199999999999997</v>
       </c>
-      <c r="D73" s="26"/>
+      <c r="D73" s="27"/>
       <c r="F73" s="1">
         <v>6</v>
       </c>
@@ -17307,7 +17626,7 @@
       <c r="H73" s="21">
         <v>0.97599999999999998</v>
       </c>
-      <c r="I73" s="26"/>
+      <c r="I73" s="27"/>
       <c r="K73" s="1">
         <v>6</v>
       </c>
@@ -17317,7 +17636,7 @@
       <c r="M73" s="21">
         <v>0.876</v>
       </c>
-      <c r="N73" s="26"/>
+      <c r="N73" s="27"/>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
@@ -17329,7 +17648,7 @@
       <c r="C74" s="21">
         <v>0.82199999999999995</v>
       </c>
-      <c r="D74" s="26"/>
+      <c r="D74" s="27"/>
       <c r="F74" s="1">
         <v>7</v>
       </c>
@@ -17339,7 +17658,7 @@
       <c r="H74" s="21">
         <v>0.97599999999999998</v>
       </c>
-      <c r="I74" s="26"/>
+      <c r="I74" s="27"/>
       <c r="K74" s="1">
         <v>7</v>
       </c>
@@ -17349,7 +17668,7 @@
       <c r="M74" s="21">
         <v>0.89300000000000002</v>
       </c>
-      <c r="N74" s="26"/>
+      <c r="N74" s="27"/>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
@@ -17361,7 +17680,7 @@
       <c r="C75" s="21">
         <v>0.82399999999999995</v>
       </c>
-      <c r="D75" s="26"/>
+      <c r="D75" s="27"/>
       <c r="F75" s="1">
         <v>8</v>
       </c>
@@ -17371,7 +17690,7 @@
       <c r="H75" s="21">
         <v>0.91800000000000004</v>
       </c>
-      <c r="I75" s="26"/>
+      <c r="I75" s="27"/>
       <c r="K75" s="1">
         <v>8</v>
       </c>
@@ -17381,7 +17700,7 @@
       <c r="M75" s="21">
         <v>0.98799999999999999</v>
       </c>
-      <c r="N75" s="26"/>
+      <c r="N75" s="27"/>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
@@ -17393,7 +17712,7 @@
       <c r="C76" s="21">
         <v>0.92500000000000004</v>
       </c>
-      <c r="D76" s="26"/>
+      <c r="D76" s="27"/>
       <c r="F76" s="1">
         <v>9</v>
       </c>
@@ -17403,7 +17722,7 @@
       <c r="H76" s="21">
         <v>0.97899999999999998</v>
       </c>
-      <c r="I76" s="26"/>
+      <c r="I76" s="27"/>
       <c r="K76" s="1">
         <v>9</v>
       </c>
@@ -17413,7 +17732,7 @@
       <c r="M76" s="21">
         <v>0.89500000000000002</v>
       </c>
-      <c r="N76" s="26"/>
+      <c r="N76" s="27"/>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
@@ -17425,7 +17744,7 @@
       <c r="C77" s="21">
         <v>0.83199999999999996</v>
       </c>
-      <c r="D77" s="26"/>
+      <c r="D77" s="27"/>
       <c r="F77" s="1">
         <v>10</v>
       </c>
@@ -17435,7 +17754,7 @@
       <c r="H77" s="21">
         <v>0.97599999999999998</v>
       </c>
-      <c r="I77" s="26"/>
+      <c r="I77" s="27"/>
       <c r="K77" s="1">
         <v>10</v>
       </c>
@@ -17445,7 +17764,7 @@
       <c r="M77" s="21">
         <v>0.98199999999999998</v>
       </c>
-      <c r="N77" s="26"/>
+      <c r="N77" s="27"/>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
@@ -17457,7 +17776,7 @@
       <c r="C78" s="21">
         <v>0.82899999999999996</v>
       </c>
-      <c r="D78" s="26"/>
+      <c r="D78" s="27"/>
       <c r="F78" s="1">
         <v>11</v>
       </c>
@@ -17467,7 +17786,7 @@
       <c r="H78" s="21">
         <v>0.94899999999999995</v>
       </c>
-      <c r="I78" s="26"/>
+      <c r="I78" s="27"/>
       <c r="K78" s="1">
         <v>11</v>
       </c>
@@ -17477,7 +17796,7 @@
       <c r="M78" s="21">
         <v>0.98099999999999998</v>
       </c>
-      <c r="N78" s="26"/>
+      <c r="N78" s="27"/>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
@@ -17489,7 +17808,7 @@
       <c r="C79" s="21">
         <v>0.95399999999999996</v>
       </c>
-      <c r="D79" s="26"/>
+      <c r="D79" s="27"/>
       <c r="F79" s="1">
         <v>12</v>
       </c>
@@ -17499,7 +17818,7 @@
       <c r="H79" s="21">
         <v>0.99299999999999999</v>
       </c>
-      <c r="I79" s="26"/>
+      <c r="I79" s="27"/>
       <c r="K79" s="1">
         <v>12</v>
       </c>
@@ -17509,7 +17828,7 @@
       <c r="M79" s="21">
         <v>0.95899999999999996</v>
       </c>
-      <c r="N79" s="26"/>
+      <c r="N79" s="27"/>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
@@ -17550,7 +17869,7 @@
       <c r="C99" s="21">
         <v>0.92200000000000004</v>
       </c>
-      <c r="D99" s="26" t="s">
+      <c r="D99" s="27" t="s">
         <v>28</v>
       </c>
       <c r="F99" s="1">
@@ -17562,7 +17881,7 @@
       <c r="H99" s="21">
         <v>0.874</v>
       </c>
-      <c r="I99" s="26" t="s">
+      <c r="I99" s="27" t="s">
         <v>29</v>
       </c>
       <c r="K99" s="1">
@@ -17574,7 +17893,7 @@
       <c r="M99" s="21">
         <v>0.99299999999999999</v>
       </c>
-      <c r="N99" s="26" t="s">
+      <c r="N99" s="27" t="s">
         <v>30</v>
       </c>
     </row>
@@ -17588,7 +17907,7 @@
       <c r="C100" s="21">
         <v>0.91600000000000004</v>
       </c>
-      <c r="D100" s="26"/>
+      <c r="D100" s="27"/>
       <c r="F100" s="1">
         <v>1</v>
       </c>
@@ -17598,7 +17917,7 @@
       <c r="H100" s="21">
         <v>0.89500000000000002</v>
       </c>
-      <c r="I100" s="26"/>
+      <c r="I100" s="27"/>
       <c r="K100" s="1">
         <v>1</v>
       </c>
@@ -17608,7 +17927,7 @@
       <c r="M100" s="21">
         <v>0.98499999999999999</v>
       </c>
-      <c r="N100" s="26"/>
+      <c r="N100" s="27"/>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
@@ -17620,7 +17939,7 @@
       <c r="C101" s="21">
         <v>0.89200000000000002</v>
       </c>
-      <c r="D101" s="26"/>
+      <c r="D101" s="27"/>
       <c r="F101" s="1">
         <v>2</v>
       </c>
@@ -17630,7 +17949,7 @@
       <c r="H101" s="21">
         <v>0.96299999999999997</v>
       </c>
-      <c r="I101" s="26"/>
+      <c r="I101" s="27"/>
       <c r="K101" s="1">
         <v>2</v>
       </c>
@@ -17640,7 +17959,7 @@
       <c r="M101" s="21">
         <v>0.96699999999999997</v>
       </c>
-      <c r="N101" s="26"/>
+      <c r="N101" s="27"/>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
@@ -17652,7 +17971,7 @@
       <c r="C102" s="21">
         <v>0.91</v>
       </c>
-      <c r="D102" s="26"/>
+      <c r="D102" s="27"/>
       <c r="F102" s="1">
         <v>3</v>
       </c>
@@ -17662,7 +17981,7 @@
       <c r="H102" s="21">
         <v>0.97199999999999998</v>
       </c>
-      <c r="I102" s="26"/>
+      <c r="I102" s="27"/>
       <c r="K102" s="1">
         <v>3</v>
       </c>
@@ -17672,7 +17991,7 @@
       <c r="M102" s="21">
         <v>0.995</v>
       </c>
-      <c r="N102" s="26"/>
+      <c r="N102" s="27"/>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
@@ -17684,7 +18003,7 @@
       <c r="C103" s="21">
         <v>0.89800000000000002</v>
       </c>
-      <c r="D103" s="26"/>
+      <c r="D103" s="27"/>
       <c r="F103" s="1">
         <v>4</v>
       </c>
@@ -17694,7 +18013,7 @@
       <c r="H103" s="21">
         <v>0.98399999999999999</v>
       </c>
-      <c r="I103" s="26"/>
+      <c r="I103" s="27"/>
       <c r="K103" s="1">
         <v>4</v>
       </c>
@@ -17704,7 +18023,7 @@
       <c r="M103" s="21">
         <v>0.98699999999999999</v>
       </c>
-      <c r="N103" s="26"/>
+      <c r="N103" s="27"/>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
@@ -17716,7 +18035,7 @@
       <c r="C104" s="21">
         <v>0.88</v>
       </c>
-      <c r="D104" s="26"/>
+      <c r="D104" s="27"/>
       <c r="F104" s="1">
         <v>5</v>
       </c>
@@ -17726,7 +18045,7 @@
       <c r="H104" s="21">
         <v>0.98299999999999998</v>
       </c>
-      <c r="I104" s="26"/>
+      <c r="I104" s="27"/>
       <c r="K104" s="1">
         <v>5</v>
       </c>
@@ -17736,7 +18055,7 @@
       <c r="M104" s="21">
         <v>0.996</v>
       </c>
-      <c r="N104" s="26"/>
+      <c r="N104" s="27"/>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
@@ -17748,7 +18067,7 @@
       <c r="C105" s="21">
         <v>0.90400000000000003</v>
       </c>
-      <c r="D105" s="26"/>
+      <c r="D105" s="27"/>
       <c r="F105" s="1">
         <v>6</v>
       </c>
@@ -17758,7 +18077,7 @@
       <c r="H105" s="21">
         <v>0.98299999999999998</v>
       </c>
-      <c r="I105" s="26"/>
+      <c r="I105" s="27"/>
       <c r="K105" s="1">
         <v>6</v>
       </c>
@@ -17768,7 +18087,7 @@
       <c r="M105" s="21">
         <v>0.99299999999999999</v>
       </c>
-      <c r="N105" s="26"/>
+      <c r="N105" s="27"/>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
@@ -17780,7 +18099,7 @@
       <c r="C106" s="21">
         <v>0.96699999999999997</v>
       </c>
-      <c r="D106" s="26"/>
+      <c r="D106" s="27"/>
       <c r="F106" s="1">
         <v>7</v>
       </c>
@@ -17790,7 +18109,7 @@
       <c r="H106" s="21">
         <v>0.98299999999999998</v>
       </c>
-      <c r="I106" s="26"/>
+      <c r="I106" s="27"/>
       <c r="K106" s="1">
         <v>7</v>
       </c>
@@ -17800,7 +18119,7 @@
       <c r="M106" s="21">
         <v>0.98899999999999999</v>
       </c>
-      <c r="N106" s="26"/>
+      <c r="N106" s="27"/>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
@@ -17812,7 +18131,7 @@
       <c r="C107" s="21">
         <v>0.97399999999999998</v>
       </c>
-      <c r="D107" s="26"/>
+      <c r="D107" s="27"/>
       <c r="F107" s="1">
         <v>8</v>
       </c>
@@ -17822,7 +18141,7 @@
       <c r="H107" s="21">
         <v>0.98899999999999999</v>
       </c>
-      <c r="I107" s="26"/>
+      <c r="I107" s="27"/>
       <c r="K107" s="1">
         <v>8</v>
       </c>
@@ -17832,7 +18151,7 @@
       <c r="M107" s="21">
         <v>0.96099999999999997</v>
       </c>
-      <c r="N107" s="26"/>
+      <c r="N107" s="27"/>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
@@ -17844,7 +18163,7 @@
       <c r="C108" s="21">
         <v>0.97799999999999998</v>
       </c>
-      <c r="D108" s="26"/>
+      <c r="D108" s="27"/>
       <c r="F108" s="1">
         <v>9</v>
       </c>
@@ -17854,7 +18173,7 @@
       <c r="H108" s="21">
         <v>0.89900000000000002</v>
       </c>
-      <c r="I108" s="26"/>
+      <c r="I108" s="27"/>
       <c r="K108" s="1">
         <v>9</v>
       </c>
@@ -17864,7 +18183,7 @@
       <c r="M108" s="21">
         <v>0.96</v>
       </c>
-      <c r="N108" s="26"/>
+      <c r="N108" s="27"/>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
@@ -17876,7 +18195,7 @@
       <c r="C109" s="21">
         <v>0.97699999999999998</v>
       </c>
-      <c r="D109" s="26"/>
+      <c r="D109" s="27"/>
       <c r="F109" s="1">
         <v>10</v>
       </c>
@@ -17886,7 +18205,7 @@
       <c r="H109" s="21">
         <v>0.97199999999999998</v>
       </c>
-      <c r="I109" s="26"/>
+      <c r="I109" s="27"/>
       <c r="K109" s="1">
         <v>10</v>
       </c>
@@ -17896,7 +18215,7 @@
       <c r="M109" s="21">
         <v>0.96399999999999997</v>
       </c>
-      <c r="N109" s="26"/>
+      <c r="N109" s="27"/>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
@@ -17908,7 +18227,7 @@
       <c r="C110" s="21">
         <v>0.97599999999999998</v>
       </c>
-      <c r="D110" s="26"/>
+      <c r="D110" s="27"/>
       <c r="F110" s="1">
         <v>11</v>
       </c>
@@ -17918,7 +18237,7 @@
       <c r="H110" s="21">
         <v>0.85599999999999998</v>
       </c>
-      <c r="I110" s="26"/>
+      <c r="I110" s="27"/>
       <c r="K110" s="1">
         <v>11</v>
       </c>
@@ -17928,7 +18247,7 @@
       <c r="M110" s="21">
         <v>0.96</v>
       </c>
-      <c r="N110" s="26"/>
+      <c r="N110" s="27"/>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
@@ -17940,7 +18259,7 @@
       <c r="C111" s="21">
         <v>0.97899999999999998</v>
       </c>
-      <c r="D111" s="26"/>
+      <c r="D111" s="27"/>
       <c r="F111" s="1">
         <v>12</v>
       </c>
@@ -17950,7 +18269,7 @@
       <c r="H111" s="21">
         <v>0.97399999999999998</v>
       </c>
-      <c r="I111" s="26"/>
+      <c r="I111" s="27"/>
       <c r="K111" s="1">
         <v>12</v>
       </c>
@@ -17960,22 +18279,22 @@
       <c r="M111" s="21">
         <v>0.96599999999999997</v>
       </c>
-      <c r="N111" s="26"/>
+      <c r="N111" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D67:D79"/>
+    <mergeCell ref="I67:I79"/>
+    <mergeCell ref="N67:N79"/>
+    <mergeCell ref="D99:D111"/>
+    <mergeCell ref="I99:I111"/>
+    <mergeCell ref="N99:N111"/>
     <mergeCell ref="D2:D14"/>
     <mergeCell ref="I2:I14"/>
     <mergeCell ref="N2:N8"/>
     <mergeCell ref="D34:D46"/>
     <mergeCell ref="I34:I46"/>
     <mergeCell ref="N34:N46"/>
-    <mergeCell ref="D67:D79"/>
-    <mergeCell ref="I67:I79"/>
-    <mergeCell ref="N67:N79"/>
-    <mergeCell ref="D99:D111"/>
-    <mergeCell ref="I99:I111"/>
-    <mergeCell ref="N99:N111"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>